<commit_message>
added tests for under and over-sampled sensor filter loading
</commit_message>
<xml_diff>
--- a/sambuca_core/tests/data/sensor_filters/sensor_filters.xlsx
+++ b/sambuca_core/tests/data/sensor_filters/sensor_filters.xlsx
@@ -5,19 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="638" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="638" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="3_band_350_900" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="4_band_300_1000" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="5_band_400_800" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="10nm_3_bands_350_900" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="0.1nm_3_bands_350_355" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
   <si>
     <t>Band 1</t>
   </si>
@@ -38,8 +40,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -122,12 +126,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -151,7 +171,7 @@
   <dimension ref="A1:D552"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="1" sqref="E103:E152 A101"/>
+      <selection pane="topLeft" activeCell="A101" activeCellId="1" sqref="D34:D52 A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7902,8 +7922,8 @@
   </sheetPr>
   <dimension ref="A1:E702"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E103" activeCellId="0" sqref="E103:E152"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E103" activeCellId="1" sqref="D34:D52 E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -19861,7 +19881,7 @@
   <dimension ref="A1:F402"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="E103:E152 E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="D34:D52 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -27915,4 +27935,1580 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D57"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="D34:D52 B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>390</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>410</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>430</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>440</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>450</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>460</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>470</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>480</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>490</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>510</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>520</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>530</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>540</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>550</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>570</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>580</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>590</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>610</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>620</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>630</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>640</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>650</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>660</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>670</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>680</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>690</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>710</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>720</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>730</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>740</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>750</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>760</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>770</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>780</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>790</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>800</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>810</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>820</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>830</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>840</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>850</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>860</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>870</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>880</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>890</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>900</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D52"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34:D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="3" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>350</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>350.1</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>350.2</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>350.3</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>350.4</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>350.5</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>350.6</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>350.7</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>350.8</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>350.9</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>351</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>351.1</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>351.2</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>351.3</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>351.4</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>351.5</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>351.6</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>351.7</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>351.8</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>351.9</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>352</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>352.1</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>352.200000000001</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>352.3</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>352.400000000001</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>352.500000000001</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>352.600000000001</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>352.700000000001</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>352.800000000001</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>352.900000000001</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>353.000000000001</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>353.100000000001</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>353.200000000001</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>353.300000000001</v>
+      </c>
+      <c r="B35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>353.400000000001</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>353.500000000001</v>
+      </c>
+      <c r="B37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>353.600000000001</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>353.700000000001</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>353.800000000001</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>353.900000000001</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
+        <v>354.000000000001</v>
+      </c>
+      <c r="B42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="n">
+        <v>354.100000000001</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="n">
+        <v>354.200000000001</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="n">
+        <v>354.300000000001</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="n">
+        <v>354.400000000001</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="n">
+        <v>354.500000000001</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="n">
+        <v>354.600000000001</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="n">
+        <v>354.700000000001</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="n">
+        <v>354.800000000001</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="n">
+        <v>354.900000000001</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="n">
+        <v>355.000000000001</v>
+      </c>
+      <c r="B52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated sensor filter normalisation test so that it doesn't assume that each band contains duplicate values
</commit_message>
<xml_diff>
--- a/sambuca_core/tests/data/sensor_filters/sensor_filters.xlsx
+++ b/sambuca_core/tests/data/sensor_filters/sensor_filters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="638" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="587" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="3_band_350_900" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,8 +53,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -137,7 +137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,20 +146,16 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -181,8 +177,8 @@
   </sheetPr>
   <dimension ref="A1:D552"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="A61:A65 A38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -304,7 +300,7 @@
         <v>357</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>0.43</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2</v>
@@ -338,7 +334,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,7 +342,7 @@
         <v>360</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2</v>
@@ -380,7 +376,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3</v>
+        <v>3.562</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +384,7 @@
         <v>363</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2</v>
@@ -405,7 +401,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>2</v>
+        <v>2.39</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>3</v>
@@ -430,7 +426,7 @@
         <v>366</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
@@ -486,10 +482,10 @@
         <v>370</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1</v>
+        <v>4.3</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>3</v>
@@ -542,7 +538,7 @@
         <v>374</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>2</v>
@@ -632,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7934,7 +7930,7 @@
   <dimension ref="A1:E702"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E103" activeCellId="1" sqref="A61:A65 E103"/>
+      <selection pane="topLeft" activeCell="E103" activeCellId="0" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -19892,7 +19888,7 @@
   <dimension ref="A1:F402"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="A61:A65 E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -27956,7 +27952,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="A61:A65 B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -28778,738 +28774,736 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B56" activeCellId="1" sqref="A61:A65 B56"/>
+      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="3" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="3" t="n">
         <v>350</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="3" t="n">
         <v>350.1</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="3" t="n">
         <v>350.2</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>0.8</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="3" t="n">
         <v>350.3</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="n">
+      <c r="B5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="3" t="n">
         <v>350.4</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="n">
+      <c r="B6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="3" t="n">
         <v>350.5</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="3" t="n">
         <v>350.6</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="4" t="n">
         <v>0.7</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="3" t="n">
         <v>350.7</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="3" t="n">
         <v>350.8</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>0.2</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="3" t="n">
         <v>350.9</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>0.15</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="3" t="n">
         <v>351</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="3" t="n">
         <v>351.1</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="4" t="n">
         <v>0.2</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="3" t="n">
         <v>351.2</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="3" t="n">
         <v>351.3</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="3" t="n">
         <v>351.4</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="3" t="n">
         <v>351.5</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="3" t="n">
         <v>351.6</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="3" t="n">
         <v>351.7</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="3" t="n">
         <v>351.8</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="4" t="n">
         <v>0.7</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="3" t="n">
         <v>351.9</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="4" t="n">
         <v>0.8</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="3" t="n">
         <v>352</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="3" t="n">
         <v>352.1</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="3" t="n">
         <v>352.200000000001</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="4" t="n">
         <v>0.8</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="3" t="n">
         <v>352.3</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="3" t="n">
         <v>352.400000000001</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="4" t="n">
         <v>0.35</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="3" t="n">
         <v>352.500000000001</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="4" t="n">
         <v>0.2</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="3" t="n">
         <v>352.600000000001</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="3" t="n">
         <v>352.700000000001</v>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="4" t="n">
         <v>0.15</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="3" t="n">
         <v>352.800000000001</v>
       </c>
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="4" t="n">
         <v>0.05</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="3" t="n">
         <v>352.900000000001</v>
       </c>
-      <c r="B31" s="3" t="n">
+      <c r="B31" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="3" t="n">
         <v>353.000000000001</v>
       </c>
-      <c r="B32" s="3" t="n">
+      <c r="B32" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D32" s="3" t="n">
+      <c r="D32" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="3" t="n">
         <v>353.100000000001</v>
       </c>
-      <c r="B33" s="3" t="n">
+      <c r="B33" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="3" t="n">
         <v>353.200000000001</v>
       </c>
-      <c r="B34" s="3" t="n">
+      <c r="B34" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D34" s="3" t="n">
+      <c r="D34" s="4" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="3" t="n">
         <v>353.300000000001</v>
       </c>
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D35" s="3" t="n">
+      <c r="D35" s="4" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="3" t="n">
         <v>353.400000000001</v>
       </c>
-      <c r="B36" s="3" t="n">
+      <c r="B36" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="4" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="3" t="n">
         <v>353.500000000001</v>
       </c>
-      <c r="B37" s="3" t="n">
+      <c r="B37" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="4" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="3" t="n">
         <v>353.600000000001</v>
       </c>
-      <c r="B38" s="3" t="n">
+      <c r="B38" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="4" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
+      <c r="A39" s="3" t="n">
         <v>353.700000000001</v>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="4" t="n">
         <v>0.6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
+      <c r="A40" s="3" t="n">
         <v>353.800000000001</v>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="4" t="n">
         <v>0.6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
+      <c r="A41" s="3" t="n">
         <v>353.900000000001</v>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="4" t="n">
         <v>0.6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
+      <c r="A42" s="3" t="n">
         <v>354.000000000001</v>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="4" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
+      <c r="A43" s="3" t="n">
         <v>354.100000000001</v>
       </c>
-      <c r="B43" s="3" t="n">
+      <c r="B43" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D43" s="3" t="n">
+      <c r="D43" s="4" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
+      <c r="A44" s="3" t="n">
         <v>354.200000000001</v>
       </c>
-      <c r="B44" s="3" t="n">
+      <c r="B44" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C44" s="3" t="n">
+      <c r="C44" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D44" s="3" t="n">
+      <c r="D44" s="4" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="n">
+      <c r="A45" s="3" t="n">
         <v>354.300000000001</v>
       </c>
-      <c r="B45" s="3" t="n">
+      <c r="B45" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D45" s="3" t="n">
+      <c r="D45" s="4" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="n">
+      <c r="A46" s="3" t="n">
         <v>354.400000000001</v>
       </c>
-      <c r="B46" s="3" t="n">
+      <c r="B46" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D46" s="3" t="n">
+      <c r="D46" s="4" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
+      <c r="A47" s="3" t="n">
         <v>354.500000000001</v>
       </c>
-      <c r="B47" s="3" t="n">
+      <c r="B47" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C47" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D47" s="3" t="n">
+      <c r="D47" s="4" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
+      <c r="A48" s="3" t="n">
         <v>354.600000000001</v>
       </c>
-      <c r="B48" s="3" t="n">
+      <c r="B48" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C48" s="3" t="n">
+      <c r="C48" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D48" s="3" t="n">
+      <c r="D48" s="4" t="n">
         <v>0.35</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
+      <c r="A49" s="3" t="n">
         <v>354.700000000001</v>
       </c>
-      <c r="B49" s="3" t="n">
+      <c r="B49" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C49" s="3" t="n">
+      <c r="C49" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D49" s="3" t="n">
+      <c r="D49" s="4" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="n">
+      <c r="A50" s="3" t="n">
         <v>354.800000000001</v>
       </c>
-      <c r="B50" s="3" t="n">
+      <c r="B50" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C50" s="3" t="n">
+      <c r="C50" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D50" s="3" t="n">
+      <c r="D50" s="4" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="n">
+      <c r="A51" s="3" t="n">
         <v>354.900000000001</v>
       </c>
-      <c r="B51" s="3" t="n">
+      <c r="B51" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C51" s="3" t="n">
+      <c r="C51" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D51" s="3" t="n">
+      <c r="D51" s="4" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
+      <c r="A52" s="3" t="n">
         <v>355.000000000001</v>
       </c>
-      <c r="B52" s="3" t="n">
+      <c r="B52" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C52" s="3" t="n">
+      <c r="C52" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D52" s="3" t="n">
+      <c r="D52" s="4" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -29532,7 +29526,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="A61:A65 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -29619,8 +29613,8 @@
   </sheetPr>
   <dimension ref="A1:D552"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61:A65"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>